<commit_message>
updated condition description for madrob and beast
</commit_message>
<xml_diff>
--- a/data/madrob/madrob-v4.0.xlsx
+++ b/data/madrob/madrob-v4.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="166">
   <si>
     <t xml:space="preserve">Scenario-Protocol-PI-PI Algo template</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t xml:space="preserve">the side of the door that the robot must reach by going through the door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disturbance type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The profile of breaking action applied to the door panel based on its angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[No Force, Constant Force, Sudden Force, Sudden Ramp, Wind Ramp]</t>
   </si>
   <si>
     <t xml:space="preserve">Testbed</t>
@@ -2502,8 +2514,8 @@
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2785,29 +2797,39 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="24"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="28" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
@@ -2816,13 +2838,13 @@
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="25"/>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
@@ -2866,31 +2888,31 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D33" s="36"/>
       <c r="E33" s="36"/>
       <c r="F33" s="36"/>
       <c r="G33" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="24"/>
       <c r="B34" s="37" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C34" s="37" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
@@ -2901,10 +2923,10 @@
         <v>0</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -2915,10 +2937,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -2929,10 +2951,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -2943,10 +2965,10 @@
         <v>3</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
@@ -2957,10 +2979,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
@@ -2971,10 +2993,10 @@
         <v>5</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
@@ -2985,10 +3007,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
@@ -2999,10 +3021,10 @@
         <v>7</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -3013,10 +3035,10 @@
         <v>8</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
@@ -3031,51 +3053,51 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="41" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B46" s="41"/>
       <c r="C46" s="42" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D46" s="43" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
       <c r="G46" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B47" s="44"/>
       <c r="C47" s="45" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D47" s="45" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E47" s="45"/>
       <c r="F47" s="45"/>
       <c r="G47" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="44" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B48" s="44"/>
       <c r="C48" s="46" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D48" s="47"/>
       <c r="E48" s="47"/>
       <c r="F48" s="47"/>
       <c r="G48" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4087,7 +4109,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
@@ -4103,7 +4125,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B1" s="48"/>
     </row>
@@ -4121,10 +4143,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,7 +4154,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,20 +4162,20 @@
         <v>34</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>39</v>
@@ -4161,41 +4183,41 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B12" s="46"/>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,10 +4234,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4223,7 +4245,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,20 +4253,20 @@
         <v>34</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>39</v>
@@ -4252,41 +4274,41 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4303,10 +4325,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4314,7 +4336,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4322,20 +4344,20 @@
         <v>34</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B29" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B30" s="55" t="s">
         <v>39</v>
@@ -4343,41 +4365,41 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B34" s="46"/>
       <c r="C34" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4394,10 +4416,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B37" s="59" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,7 +4427,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="54" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4413,20 +4435,20 @@
         <v>34</v>
       </c>
       <c r="B39" s="54" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B41" s="55" t="s">
         <v>39</v>
@@ -4434,41 +4456,41 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B42" s="54" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B44" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B45" s="46"/>
       <c r="C45" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4485,10 +4507,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B48" s="59" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,7 +4518,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="54" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4504,20 +4526,20 @@
         <v>34</v>
       </c>
       <c r="B50" s="54" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B51" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B52" s="55" t="s">
         <v>39</v>
@@ -4525,41 +4547,41 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B53" s="54" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B55" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B56" s="46"/>
       <c r="C56" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4576,10 +4598,10 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B59" s="59" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4587,7 +4609,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="60" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4595,20 +4617,20 @@
         <v>34</v>
       </c>
       <c r="B61" s="60" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B62" s="60" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B63" s="55" t="s">
         <v>39</v>
@@ -4616,41 +4638,41 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B64" s="54" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B67" s="46"/>
       <c r="C67" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4667,10 +4689,10 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B70" s="59" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4678,7 +4700,7 @@
         <v>10</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4686,20 +4708,20 @@
         <v>34</v>
       </c>
       <c r="B72" s="54" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B73" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B74" s="55" t="s">
         <v>39</v>
@@ -4707,41 +4729,41 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B75" s="54" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B76" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B77" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B78" s="46"/>
       <c r="C78" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4758,10 +4780,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B81" s="59" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4769,7 +4791,7 @@
         <v>10</v>
       </c>
       <c r="B82" s="54" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4782,15 +4804,15 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="52" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B84" s="54" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="52" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B85" s="54" t="s">
         <v>39</v>
@@ -4798,41 +4820,41 @@
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B86" s="54" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B87" s="42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B88" s="58" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="57" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B89" s="46"/>
       <c r="C89" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4841,7 +4863,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="61" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B91" s="61"/>
     </row>
@@ -4859,7 +4881,7 @@
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="64" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B94" s="65" t="s">
         <v>28</v>
@@ -4870,12 +4892,12 @@
         <v>10</v>
       </c>
       <c r="B95" s="66" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="64" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B96" s="66" t="s">
         <v>39</v>
@@ -4883,53 +4905,53 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="64" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B97" s="67" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="64" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B98" s="64" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="64" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B99" s="66" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="64" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B100" s="66" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="64" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B101" s="66" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C101" s="68" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="64" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B102" s="66" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4942,50 +4964,50 @@
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="52" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B104" s="54" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="52" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B105" s="54" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="52" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B106" s="54" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="52" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B107" s="54" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="52" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B108" s="54" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="52" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B109" s="54" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4994,11 +5016,11 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="69" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B112" s="69"/>
       <c r="C112" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5006,59 +5028,59 @@
         <v>6</v>
       </c>
       <c r="B113" s="71" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C113" s="2"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="72" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B114" s="46" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C114" s="2"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="72" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B115" s="46"/>
       <c r="C115" s="2"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="72" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B116" s="54" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C116" s="2"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="72" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B117" s="46" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C117" s="2"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="72" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B118" s="73" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C118" s="2"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="72" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B119" s="54" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C119" s="2"/>
     </row>
@@ -5900,7 +5922,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="74" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -5915,18 +5937,18 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -5937,48 +5959,48 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>

</xml_diff>

<commit_message>
updated conditions description of madrob (again)
</commit_message>
<xml_diff>
--- a/data/madrob/madrob-v4.0.xlsx
+++ b/data/madrob/madrob-v4.0.xlsx
@@ -151,7 +151,7 @@
     <t xml:space="preserve">destination side</t>
   </si>
   <si>
-    <t xml:space="preserve">the side of the door that the robot must reach by going through the door</t>
+    <t xml:space="preserve">the side of the door that the robot must reach by going through the door (opposite of the approach side)</t>
   </si>
   <si>
     <t xml:space="preserve">disturbance type</t>
@@ -2514,8 +2514,8 @@
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2774,7 +2774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24"/>
       <c r="B24" s="11" t="s">
         <v>41</v>

</xml_diff>